<commit_message>
changes since last meeting
</commit_message>
<xml_diff>
--- a/ProjectManagement/Phase 1 Requirements.xlsx
+++ b/ProjectManagement/Phase 1 Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DS\f\02_Preaching\04 Preaching Software\Project Management\Phase 1\PreachingAssistant\ProjectManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hariksetra\Desktop\FromHariksetraPrabhu\fwdpreachingsoftwarerequirementsdocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>X</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t xml:space="preserve">Android, JBOSS, SVN or GIT, MySQL, Hybrid APP, Phone Gap, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anjular JS, IONIX, JAVA, Spring Boot, Tomcat/Jetty, </t>
+  </si>
+  <si>
+    <t>Sprint Management</t>
   </si>
 </sst>
 </file>
@@ -166,11 +172,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -234,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -269,7 +275,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="131" workbookViewId="0">
-      <selection sqref="A1:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="131" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,28 +473,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -497,8 +503,8 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -509,8 +515,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -521,8 +527,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -533,8 +539,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -543,8 +549,8 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -555,8 +561,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -565,16 +571,16 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -583,8 +589,8 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -595,8 +601,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -607,8 +613,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -619,8 +625,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -631,8 +637,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -643,8 +649,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="1"/>
@@ -653,16 +659,16 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -671,8 +677,8 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -681,10 +687,10 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
@@ -697,6 +703,16 @@
         <v>0</v>
       </c>
       <c r="D22" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>